<commit_message>
Actually fixed stuff this time (ignore the last commit)
</commit_message>
<xml_diff>
--- a/SwimProgress.xlsx
+++ b/SwimProgress.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8805" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="100 BK" sheetId="1" r:id="rId1"/>
-    <sheet name="50 FR" sheetId="2" r:id="rId2"/>
+    <sheet name="200 BK" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -127,7 +127,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -902,7 +901,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1831,12 +1829,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1844,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43505</v>
       </c>
@@ -1852,7 +1850,7 @@
         <v>6.8379629629629639E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43492</v>
       </c>
@@ -1860,7 +1858,7 @@
         <v>7.023148148148149E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43443</v>
       </c>
@@ -1868,7 +1866,7 @@
         <v>6.9884259259259259E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43435</v>
       </c>
@@ -1876,7 +1874,7 @@
         <v>7.1134259259259252E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43422</v>
       </c>
@@ -1884,7 +1882,7 @@
         <v>7.0740740740740736E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43408</v>
       </c>
@@ -1892,7 +1890,7 @@
         <v>7.1284722222222225E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43394</v>
       </c>
@@ -1900,7 +1898,7 @@
         <v>7.1122685185185189E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43274</v>
       </c>
@@ -1908,7 +1906,7 @@
         <v>7.1493055555555557E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43141</v>
       </c>
@@ -1916,7 +1914,7 @@
         <v>7.2268518518518515E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43127</v>
       </c>
@@ -1924,7 +1922,7 @@
         <v>7.2523148148148154E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43113</v>
       </c>
@@ -1932,7 +1930,7 @@
         <v>7.2905092592592596E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43078</v>
       </c>
@@ -1940,7 +1938,7 @@
         <v>7.5694444444444453E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43058</v>
       </c>
@@ -1948,7 +1946,7 @@
         <v>7.4409722222222206E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43044</v>
       </c>
@@ -1956,7 +1954,7 @@
         <v>7.2766203703703708E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43030</v>
       </c>
@@ -1964,7 +1962,7 @@
         <v>7.4143518518518525E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42861</v>
       </c>
@@ -1972,7 +1970,7 @@
         <v>7.7685185185185192E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42777</v>
       </c>
@@ -1980,7 +1978,7 @@
         <v>7.6412037037037041E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42707</v>
       </c>
@@ -1988,7 +1986,7 @@
         <v>7.6631944444444436E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42686</v>
       </c>
@@ -1996,7 +1994,7 @@
         <v>7.8796296296296297E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42498</v>
       </c>
@@ -2004,7 +2002,7 @@
         <v>8.2037037037037029E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42421</v>
       </c>
@@ -2012,7 +2010,7 @@
         <v>8.226851851851853E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42406</v>
       </c>
@@ -2020,7 +2018,7 @@
         <v>8.2187500000000001E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42343</v>
       </c>
@@ -2028,7 +2026,7 @@
         <v>8.2233796296296297E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42330</v>
       </c>
@@ -2036,7 +2034,7 @@
         <v>8.2881944444444442E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>42308</v>
       </c>
@@ -2044,7 +2042,7 @@
         <v>8.59375E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42287</v>
       </c>
@@ -2052,7 +2050,7 @@
         <v>8.7094907407407401E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42133</v>
       </c>
@@ -2060,7 +2058,7 @@
         <v>8.8032407407407417E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42057</v>
       </c>
@@ -2068,7 +2066,7 @@
         <v>9.3287037037037036E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>41986</v>
       </c>
@@ -2076,7 +2074,7 @@
         <v>9.5567129629629637E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>41966</v>
       </c>
@@ -2084,7 +2082,7 @@
         <v>9.3784722222222229E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>41951</v>
       </c>
@@ -2092,7 +2090,7 @@
         <v>9.7766203703703708E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>41769</v>
       </c>
@@ -2100,7 +2098,7 @@
         <v>9.6493055555555557E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>41678</v>
       </c>
@@ -2108,7 +2106,7 @@
         <v>1.0105324074074075E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>41671</v>
       </c>
@@ -2116,7 +2114,7 @@
         <v>1.0287037037037038E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>41602</v>
       </c>
@@ -2124,7 +2122,7 @@
         <v>1.0347222222222222E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>41412</v>
       </c>
@@ -2132,7 +2130,7 @@
         <v>1.1315972222222224E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>41321</v>
       </c>
@@ -2140,7 +2138,7 @@
         <v>1.1196759259259261E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>41293</v>
       </c>
@@ -2148,7 +2146,7 @@
         <v>1.1741898148148148E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>41252</v>
       </c>
@@ -2156,7 +2154,7 @@
         <v>1.1172453703703704E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>41223</v>
       </c>
@@ -2164,178 +2162,178 @@
         <v>1.1883101851851853E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="2"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="2"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="2"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="2"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="2"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="2"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="2"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="2"/>
     </row>
   </sheetData>
@@ -2353,9 +2351,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2363,301 +2361,301 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="2"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="2"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="2"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="2"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="2"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="2"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="2"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="2"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="2"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 200 BK graph
</commit_message>
<xml_diff>
--- a/SwimProgress.xlsx
+++ b/SwimProgress.xlsx
@@ -127,6 +127,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -901,6 +902,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -929,6 +931,672 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:miter lim="800000"/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>200 Back</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'200 BK'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'200 BK'!$A$2:$A$24</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>43506</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43442</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43421</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43407</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43393</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43274</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43114</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43057</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43043</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42862</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42778</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42771</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42687</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42420</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42407</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42344</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42309</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42288</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42056</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42049</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42036</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41987</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'200 BK'!$B$2:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.00</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>1.5211805555555558E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5482638888888887E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5797453703703705E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5776620370370371E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5922453703703704E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6796296296296297E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5945601851851852E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6064814814814815E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6151620370370371E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6261574074074075E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6837962962962961E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6837962962962961E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6888888888888889E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7206018518518518E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.7949074074074074E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8628472222222223E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8180555555555554E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.9203703703703702E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9070601851851852E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.0223379629629632E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9415509259259258E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0090277777777775E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.044328703703704E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6EB5-4D17-824C-AC1A67FB598C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1968356128"/>
+        <c:axId val="1968347808"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'200 BK'!$A$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Date</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'200 BK'!$A$2:$A$24</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>m/d/yyyy</c:formatCode>
+                      <c:ptCount val="23"/>
+                      <c:pt idx="0">
+                        <c:v>43506</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>43442</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>43421</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>43407</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>43393</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>43274</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>43142</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>43114</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>43057</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>43043</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>42862</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>42778</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>42771</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>42687</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>42420</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>42407</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>42344</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>42309</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>42288</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>42056</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>42049</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>42036</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>41987</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'200 BK'!$A$2:$A$24</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>m/d/yyyy</c:formatCode>
+                      <c:ptCount val="23"/>
+                      <c:pt idx="0">
+                        <c:v>43506</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>43442</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>43421</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>43407</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>43393</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>43274</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>43142</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>43114</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>43057</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>43043</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>42862</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>42778</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>42771</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>42687</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>42420</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>42407</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>42344</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>42309</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>42288</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>42056</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>42049</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>42036</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>41987</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-6EB5-4D17-824C-AC1A67FB598C}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1968356128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1968347808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1968347808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2.1000000000000003E-3"/>
+          <c:min val="1.3000000000000004E-3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="mm:ss.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1968356128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0000000000000003E-4"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1009,7 +1677,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1543,6 +2767,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133731</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>43053</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1831,7 +3090,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2348,10 +3607,13 @@
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2362,96 +3624,211 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
+      <c r="A2" s="1">
+        <v>43506</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.5211805555555558E-3</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
+      <c r="A3" s="1">
+        <v>43442</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.5482638888888887E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
+      <c r="A4" s="1">
+        <v>43421</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.5797453703703705E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
+      <c r="A5" s="1">
+        <v>43407</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.5776620370370371E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
+      <c r="A6" s="1">
+        <v>43393</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.5922453703703704E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
+      <c r="A7" s="1">
+        <v>43274</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.6796296296296297E-3</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="A8" s="1">
+        <v>43142</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.5945601851851852E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
+      <c r="A9" s="1">
+        <v>43114</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.6064814814814815E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="A10" s="1">
+        <v>43057</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.6151620370370371E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="A11" s="1">
+        <v>43043</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.6261574074074075E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
+      <c r="A12" s="1">
+        <v>42862</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.6837962962962961E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
+      <c r="A13" s="1">
+        <v>42778</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.6837962962962961E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
+      <c r="A14" s="1">
+        <v>42771</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.6888888888888889E-3</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
+      <c r="A15" s="1">
+        <v>42687</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.7206018518518518E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>42420</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.7949074074074074E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>42407</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.8628472222222223E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>42344</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.8180555555555554E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>42309</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.9203703703703702E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>42288</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.9070601851851852E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>42056</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.0223379629629632E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>42049</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.9415509259259258E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>42036</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2.0090277777777775E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>41987</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2.044328703703704E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
@@ -2660,5 +4037,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>